<commit_message>
fix error export data
</commit_message>
<xml_diff>
--- a/public/Data Produk.xlsx
+++ b/public/Data Produk.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>No</t>
   </si>
@@ -35,31 +35,13 @@
     <t>Total Nominal</t>
   </si>
   <si>
-    <t>2023-10-22 11:03:47</t>
-  </si>
-  <si>
-    <t>Kompos</t>
-  </si>
-  <si>
-    <t>666.200,00</t>
-  </si>
-  <si>
-    <t>2023-09-04 00:00:00</t>
+    <t>2023-12-29 04:03:55</t>
+  </si>
+  <si>
+    <t>Pupuk</t>
   </si>
   <si>
     <t>0,00</t>
-  </si>
-  <si>
-    <t>2023-09-05 07:52:15</t>
-  </si>
-  <si>
-    <t>2023-09-05 08:31:19</t>
-  </si>
-  <si>
-    <t>Maggot</t>
-  </si>
-  <si>
-    <t>10.100.000,00</t>
   </si>
 </sst>
 </file>
@@ -399,7 +381,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,73 +420,13 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>211</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>2020</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>